<commit_message>
Added case for alerts for client users
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Downloads/RF.CustomExport(BaseOfExport=Reviews)[TESTING] (1).xlsx
+++ b/ADtests/Resources/Downloads/RF.CustomExport(BaseOfExport=Reviews)[TESTING] (1).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="255">
   <si>
     <t>CritID</t>
   </si>
@@ -494,13 +494,13 @@
     <t>1108. Test custom field. Number</t>
   </si>
   <si>
-    <t>278502</t>
+    <t>278541</t>
   </si>
   <si>
     <t>46.401869158879</t>
   </si>
   <si>
-    <t>2022-09-27 09:33:55</t>
+    <t>2022-09-28 10:27:53</t>
   </si>
   <si>
     <t>RF Branch 01 [Short name]</t>
@@ -536,7 +536,7 @@
     <t>2000</t>
   </si>
   <si>
-    <t>Additional info - 27.09.2022 RF</t>
+    <t>Additional info - 28.09.2022 RF</t>
   </si>
   <si>
     <t>green</t>
@@ -581,13 +581,13 @@
     <t>Approved</t>
   </si>
   <si>
-    <t>2022-09-27 09:34:07</t>
-  </si>
-  <si>
-    <t>2022-09-27 09:33:33</t>
-  </si>
-  <si>
-    <t>2022-09-27 09:33:07</t>
+    <t>2022-09-28 10:28:06</t>
+  </si>
+  <si>
+    <t>2022-09-28 10:27:28</t>
+  </si>
+  <si>
+    <t>2022-09-28 10:27:02</t>
   </si>
   <si>
     <t>122391</t>
@@ -647,7 +647,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>RF Order: Single_01 SMOKE [To check review status and answers, 27.09.2022]</t>
+    <t>RF Order: Single_01 SMOKE [To check review status and answers, 28.09.2022]</t>
   </si>
   <si>
     <t>TextB1</t>
@@ -683,133 +683,103 @@
     <t>"I AM a code" !@##%$</t>
   </si>
   <si>
-    <t>278507</t>
-  </si>
-  <si>
-    <t>2022-09-27 09:57:33</t>
-  </si>
-  <si>
-    <t>2022-09-27 10:00:54</t>
-  </si>
-  <si>
-    <t>2022-09-27 09:57:07</t>
-  </si>
-  <si>
-    <t>2022-09-27 09:56:42</t>
+    <t>278542</t>
+  </si>
+  <si>
+    <t>2022-09-28 11:25:50</t>
+  </si>
+  <si>
+    <t>2022-09-28 11:26:20</t>
+  </si>
+  <si>
+    <t>2022-09-28 11:25:19</t>
+  </si>
+  <si>
+    <t>2022-09-28 11:24:53</t>
+  </si>
+  <si>
+    <t>278565</t>
+  </si>
+  <si>
+    <t>2022-09-28 23:21:58</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>4;1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2022-09-28 23:22:13</t>
+  </si>
+  <si>
+    <t>2022-09-28 23:21:33</t>
+  </si>
+  <si>
+    <t>2022-09-28 23:21:07</t>
+  </si>
+  <si>
+    <t>278573</t>
+  </si>
+  <si>
+    <t>2022-09-29 10:44:12</t>
+  </si>
+  <si>
+    <t>Additional info - 29.09.2022 RF</t>
+  </si>
+  <si>
+    <t>2022-09-29 10:44:26</t>
+  </si>
+  <si>
+    <t>2022-09-29 10:43:47</t>
+  </si>
+  <si>
+    <t>2022-09-29 10:43:21</t>
+  </si>
+  <si>
+    <t>RF Order: Single_01 SMOKE [To check review status and answers, 29.09.2022]</t>
+  </si>
+  <si>
+    <t>278577</t>
+  </si>
+  <si>
+    <t>2022-09-29 10:59:02</t>
+  </si>
+  <si>
+    <t>2022-09-29 11:02:58</t>
+  </si>
+  <si>
+    <t>2022-09-29 10:58:36</t>
+  </si>
+  <si>
+    <t>2022-09-29 10:58:10</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>RF Order: M042 [To check send repeatedly alert, 27.09.2022]</t>
+    <t>RF Order: M042 [To check send repeatedly alert, 29.09.2022]</t>
   </si>
   <si>
     <t>RF ACTIVE project 2022 [PROJECT]</t>
   </si>
   <si>
-    <t>278514</t>
-  </si>
-  <si>
-    <t>2022-09-27 10:42:37</t>
-  </si>
-  <si>
-    <t>2022-09-27 10:47:20</t>
-  </si>
-  <si>
-    <t>2022-09-27 10:42:04</t>
-  </si>
-  <si>
-    <t>2022-09-27 10:41:39</t>
-  </si>
-  <si>
-    <t>278519</t>
-  </si>
-  <si>
-    <t>2022-09-27 12:49:41</t>
-  </si>
-  <si>
-    <t>2022-09-27 12:50:10</t>
-  </si>
-  <si>
-    <t>2022-09-27 12:48:36</t>
-  </si>
-  <si>
-    <t>2022-09-27 12:48:10</t>
-  </si>
-  <si>
-    <t>RF Order: M03 [To be accepted by a shopper and submitted with attached files, 27.09.2022]</t>
-  </si>
-  <si>
-    <t>278520</t>
-  </si>
-  <si>
-    <t>2022-09-27 12:57:01</t>
-  </si>
-  <si>
-    <t>2022-09-27 13:01:21</t>
-  </si>
-  <si>
-    <t>2022-09-27 12:56:28</t>
-  </si>
-  <si>
-    <t>2022-09-27 12:56:03</t>
-  </si>
-  <si>
-    <t>RF Order: M04 [To be returned to shopper, 27.09.2022]</t>
-  </si>
-  <si>
-    <t>278522</t>
-  </si>
-  <si>
-    <t>2022-09-27 13:10:38</t>
-  </si>
-  <si>
-    <t>2022-09-27 13:11:11</t>
-  </si>
-  <si>
-    <t>2022-09-27 13:09:33</t>
-  </si>
-  <si>
-    <t>2022-09-27 13:09:08</t>
-  </si>
-  <si>
-    <t>RF Order: M06 [To be restarted by a shopper, 27.09.2022]</t>
-  </si>
-  <si>
-    <t>278523</t>
-  </si>
-  <si>
-    <t>2022-09-27 13:18:49</t>
-  </si>
-  <si>
-    <t>2022-09-27 13:19:20</t>
-  </si>
-  <si>
-    <t>2022-09-27 13:16:38</t>
-  </si>
-  <si>
-    <t>2022-09-27 13:16:13</t>
-  </si>
-  <si>
-    <t>RF Order: M07 [To be saved and continued by shopper, 27.09.2022]</t>
-  </si>
-  <si>
-    <t>278524</t>
-  </si>
-  <si>
-    <t>2022-09-27 13:33:14</t>
-  </si>
-  <si>
-    <t>2022-09-27 13:32:09</t>
-  </si>
-  <si>
-    <t>2022-09-27 13:31:44</t>
-  </si>
-  <si>
-    <t>RF Order: S01 [Published order, (27.09.2022)]</t>
+    <t>278580</t>
+  </si>
+  <si>
+    <t>2022-09-29 12:40:43</t>
+  </si>
+  <si>
+    <t>2022-09-29 12:46:31</t>
+  </si>
+  <si>
+    <t>2022-09-29 12:40:10</t>
+  </si>
+  <si>
+    <t>2022-09-29 12:39:44</t>
   </si>
 </sst>
 </file>
@@ -1148,7 +1118,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:FG9"/>
+  <dimension ref="A1:FG7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2058,13 +2028,13 @@
         <v>207</v>
       </c>
       <c r="CP3" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="CQ3" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="CT3" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="CU3" t="s">
         <v>178</v>
@@ -2110,9 +2080,6 @@
       </c>
       <c r="FA3" t="s">
         <v>220</v>
-      </c>
-      <c r="FB3" t="s">
-        <v>230</v>
       </c>
       <c r="FC3" t="s">
         <v>221</v>
@@ -2124,13 +2091,13 @@
     </row>
     <row r="4" spans="1:163">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B4" t="s">
         <v>160</v>
       </c>
       <c r="C4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D4" t="s">
         <v>162</v>
@@ -2150,14 +2117,18 @@
       <c r="I4" t="s">
         <v>167</v>
       </c>
-      <c r="M4"/>
+      <c r="M4" t="s">
+        <v>229</v>
+      </c>
       <c r="N4" t="s">
         <v>168</v>
       </c>
       <c r="O4" t="s">
         <v>169</v>
       </c>
-      <c r="P4"/>
+      <c r="P4" t="s">
+        <v>230</v>
+      </c>
       <c r="Q4" t="s">
         <v>170</v>
       </c>
@@ -2170,7 +2141,9 @@
       <c r="AL4" t="s">
         <v>173</v>
       </c>
-      <c r="AM4"/>
+      <c r="AM4" t="s">
+        <v>231</v>
+      </c>
       <c r="AN4" t="s">
         <v>174</v>
       </c>
@@ -2238,16 +2211,16 @@
         <v>187</v>
       </c>
       <c r="BU4" t="s">
+        <v>232</v>
+      </c>
+      <c r="BV4" t="s">
+        <v>228</v>
+      </c>
+      <c r="BW4" t="s">
         <v>233</v>
       </c>
-      <c r="BV4" t="s">
-        <v>232</v>
-      </c>
-      <c r="BW4" t="s">
+      <c r="BX4" t="s">
         <v>234</v>
-      </c>
-      <c r="BX4" t="s">
-        <v>235</v>
       </c>
       <c r="BY4" t="s">
         <v>191</v>
@@ -2301,13 +2274,13 @@
         <v>207</v>
       </c>
       <c r="CP4" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="CQ4" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="CT4" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="CU4" t="s">
         <v>178</v>
@@ -2353,9 +2326,6 @@
       </c>
       <c r="FA4" t="s">
         <v>220</v>
-      </c>
-      <c r="FB4" t="s">
-        <v>230</v>
       </c>
       <c r="FC4" t="s">
         <v>221</v>
@@ -2367,13 +2337,13 @@
     </row>
     <row r="5" spans="1:163">
       <c r="A5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B5" t="s">
         <v>160</v>
       </c>
       <c r="C5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D5" t="s">
         <v>162</v>
@@ -2393,14 +2363,18 @@
       <c r="I5" t="s">
         <v>167</v>
       </c>
-      <c r="M5"/>
+      <c r="M5" t="s">
+        <v>229</v>
+      </c>
       <c r="N5" t="s">
         <v>168</v>
       </c>
       <c r="O5" t="s">
         <v>169</v>
       </c>
-      <c r="P5"/>
+      <c r="P5" t="s">
+        <v>230</v>
+      </c>
       <c r="Q5" t="s">
         <v>170</v>
       </c>
@@ -2411,9 +2385,11 @@
         <v>172</v>
       </c>
       <c r="AL5" t="s">
-        <v>173</v>
-      </c>
-      <c r="AM5"/>
+        <v>237</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>231</v>
+      </c>
       <c r="AN5" t="s">
         <v>174</v>
       </c>
@@ -2484,7 +2460,7 @@
         <v>238</v>
       </c>
       <c r="BV5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="BW5" t="s">
         <v>239</v>
@@ -2544,10 +2520,10 @@
         <v>207</v>
       </c>
       <c r="CP5" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="CQ5" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="CT5" t="s">
         <v>241</v>
@@ -2596,9 +2572,6 @@
       </c>
       <c r="FA5" t="s">
         <v>220</v>
-      </c>
-      <c r="FB5" t="s">
-        <v>230</v>
       </c>
       <c r="FC5" t="s">
         <v>221</v>
@@ -2636,14 +2609,18 @@
       <c r="I6" t="s">
         <v>167</v>
       </c>
-      <c r="M6"/>
+      <c r="M6" t="s">
+        <v>229</v>
+      </c>
       <c r="N6" t="s">
         <v>168</v>
       </c>
       <c r="O6" t="s">
         <v>169</v>
       </c>
-      <c r="P6"/>
+      <c r="P6" t="s">
+        <v>230</v>
+      </c>
       <c r="Q6" t="s">
         <v>170</v>
       </c>
@@ -2654,9 +2631,11 @@
         <v>172</v>
       </c>
       <c r="AL6" t="s">
-        <v>173</v>
-      </c>
-      <c r="AM6"/>
+        <v>237</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>231</v>
+      </c>
       <c r="AN6" t="s">
         <v>174</v>
       </c>
@@ -2787,13 +2766,13 @@
         <v>207</v>
       </c>
       <c r="CP6" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="CQ6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="CT6" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="CU6" t="s">
         <v>178</v>
@@ -2841,7 +2820,7 @@
         <v>220</v>
       </c>
       <c r="FB6" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="FC6" t="s">
         <v>221</v>
@@ -2853,13 +2832,13 @@
     </row>
     <row r="7" spans="1:163">
       <c r="A7" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B7" t="s">
         <v>160</v>
       </c>
       <c r="C7" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D7" t="s">
         <v>162</v>
@@ -2879,14 +2858,18 @@
       <c r="I7" t="s">
         <v>167</v>
       </c>
-      <c r="M7"/>
+      <c r="M7" t="s">
+        <v>229</v>
+      </c>
       <c r="N7" t="s">
         <v>168</v>
       </c>
       <c r="O7" t="s">
         <v>169</v>
       </c>
-      <c r="P7"/>
+      <c r="P7" t="s">
+        <v>230</v>
+      </c>
       <c r="Q7" t="s">
         <v>170</v>
       </c>
@@ -2897,9 +2880,11 @@
         <v>172</v>
       </c>
       <c r="AL7" t="s">
-        <v>173</v>
-      </c>
-      <c r="AM7"/>
+        <v>237</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>231</v>
+      </c>
       <c r="AN7" t="s">
         <v>174</v>
       </c>
@@ -2967,16 +2952,16 @@
         <v>187</v>
       </c>
       <c r="BU7" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="BV7" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="BW7" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="BX7" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="BY7" t="s">
         <v>191</v>
@@ -3030,13 +3015,13 @@
         <v>207</v>
       </c>
       <c r="CP7" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="CQ7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="CT7" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="CU7" t="s">
         <v>178</v>
@@ -3084,496 +3069,13 @@
         <v>220</v>
       </c>
       <c r="FB7" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="FC7" t="s">
         <v>221</v>
       </c>
       <c r="FD7"/>
       <c r="FE7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:163">
-      <c r="A8" t="s">
-        <v>254</v>
-      </c>
-      <c r="B8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C8" t="s">
-        <v>255</v>
-      </c>
-      <c r="D8" t="s">
-        <v>162</v>
-      </c>
-      <c r="E8" t="s">
-        <v>163</v>
-      </c>
-      <c r="F8" t="s">
-        <v>164</v>
-      </c>
-      <c r="G8" t="s">
-        <v>165</v>
-      </c>
-      <c r="H8" t="s">
-        <v>166</v>
-      </c>
-      <c r="I8" t="s">
-        <v>167</v>
-      </c>
-      <c r="M8"/>
-      <c r="N8" t="s">
-        <v>168</v>
-      </c>
-      <c r="O8" t="s">
-        <v>169</v>
-      </c>
-      <c r="P8"/>
-      <c r="Q8" t="s">
-        <v>170</v>
-      </c>
-      <c r="R8" t="s">
-        <v>171</v>
-      </c>
-      <c r="T8" t="s">
-        <v>172</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>173</v>
-      </c>
-      <c r="AM8"/>
-      <c r="AN8" t="s">
-        <v>174</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>175</v>
-      </c>
-      <c r="AP8"/>
-      <c r="AQ8"/>
-      <c r="AS8"/>
-      <c r="AT8" t="s">
-        <v>176</v>
-      </c>
-      <c r="AV8"/>
-      <c r="AX8" t="s">
-        <v>177</v>
-      </c>
-      <c r="AZ8" t="s">
-        <v>178</v>
-      </c>
-      <c r="BA8" t="s">
-        <v>179</v>
-      </c>
-      <c r="BB8" t="s">
-        <v>180</v>
-      </c>
-      <c r="BC8" t="s">
-        <v>181</v>
-      </c>
-      <c r="BD8" t="s">
-        <v>182</v>
-      </c>
-      <c r="BE8" t="s">
-        <v>183</v>
-      </c>
-      <c r="BG8" t="s">
-        <v>184</v>
-      </c>
-      <c r="BH8" t="s">
-        <v>185</v>
-      </c>
-      <c r="BI8"/>
-      <c r="BJ8" t="s">
-        <v>177</v>
-      </c>
-      <c r="BK8" t="s">
-        <v>178</v>
-      </c>
-      <c r="BL8" t="s">
-        <v>179</v>
-      </c>
-      <c r="BM8" t="s">
-        <v>186</v>
-      </c>
-      <c r="BN8" t="s">
-        <v>181</v>
-      </c>
-      <c r="BO8" t="s">
-        <v>182</v>
-      </c>
-      <c r="BP8" t="s">
-        <v>183</v>
-      </c>
-      <c r="BR8"/>
-      <c r="BT8" t="s">
-        <v>187</v>
-      </c>
-      <c r="BU8" t="s">
-        <v>256</v>
-      </c>
-      <c r="BV8" t="s">
-        <v>255</v>
-      </c>
-      <c r="BW8" t="s">
-        <v>257</v>
-      </c>
-      <c r="BX8" t="s">
-        <v>258</v>
-      </c>
-      <c r="BY8" t="s">
-        <v>191</v>
-      </c>
-      <c r="BZ8" t="s">
-        <v>192</v>
-      </c>
-      <c r="CA8" t="s">
-        <v>193</v>
-      </c>
-      <c r="CB8" t="s">
-        <v>194</v>
-      </c>
-      <c r="CC8" t="s">
-        <v>195</v>
-      </c>
-      <c r="CD8" t="s">
-        <v>196</v>
-      </c>
-      <c r="CE8" t="s">
-        <v>197</v>
-      </c>
-      <c r="CF8" t="s">
-        <v>198</v>
-      </c>
-      <c r="CG8" t="s">
-        <v>199</v>
-      </c>
-      <c r="CH8" t="s">
-        <v>200</v>
-      </c>
-      <c r="CI8" t="s">
-        <v>201</v>
-      </c>
-      <c r="CJ8" t="s">
-        <v>202</v>
-      </c>
-      <c r="CK8" t="s">
-        <v>203</v>
-      </c>
-      <c r="CL8" t="s">
-        <v>204</v>
-      </c>
-      <c r="CM8" t="s">
-        <v>205</v>
-      </c>
-      <c r="CN8" t="s">
-        <v>206</v>
-      </c>
-      <c r="CO8" t="s">
-        <v>207</v>
-      </c>
-      <c r="CP8" t="s">
-        <v>227</v>
-      </c>
-      <c r="CQ8" t="s">
-        <v>228</v>
-      </c>
-      <c r="CT8" t="s">
-        <v>259</v>
-      </c>
-      <c r="CU8" t="s">
-        <v>178</v>
-      </c>
-      <c r="CV8" t="s">
-        <v>211</v>
-      </c>
-      <c r="CW8" t="s">
-        <v>212</v>
-      </c>
-      <c r="CX8" t="s">
-        <v>182</v>
-      </c>
-      <c r="CY8" t="s">
-        <v>183</v>
-      </c>
-      <c r="CZ8" t="s">
-        <v>213</v>
-      </c>
-      <c r="DB8" t="s">
-        <v>214</v>
-      </c>
-      <c r="EB8" t="s">
-        <v>215</v>
-      </c>
-      <c r="ET8" t="s">
-        <v>160</v>
-      </c>
-      <c r="EU8" t="s">
-        <v>160</v>
-      </c>
-      <c r="EW8" t="s">
-        <v>216</v>
-      </c>
-      <c r="EX8" t="s">
-        <v>217</v>
-      </c>
-      <c r="EY8" t="s">
-        <v>218</v>
-      </c>
-      <c r="EZ8" t="s">
-        <v>219</v>
-      </c>
-      <c r="FA8" t="s">
-        <v>220</v>
-      </c>
-      <c r="FB8" t="s">
-        <v>230</v>
-      </c>
-      <c r="FC8" t="s">
-        <v>221</v>
-      </c>
-      <c r="FD8"/>
-      <c r="FE8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="9" spans="1:163">
-      <c r="A9" t="s">
-        <v>260</v>
-      </c>
-      <c r="B9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" t="s">
-        <v>261</v>
-      </c>
-      <c r="D9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E9" t="s">
-        <v>163</v>
-      </c>
-      <c r="F9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G9" t="s">
-        <v>165</v>
-      </c>
-      <c r="H9" t="s">
-        <v>166</v>
-      </c>
-      <c r="I9" t="s">
-        <v>167</v>
-      </c>
-      <c r="M9"/>
-      <c r="N9" t="s">
-        <v>168</v>
-      </c>
-      <c r="O9" t="s">
-        <v>169</v>
-      </c>
-      <c r="P9"/>
-      <c r="Q9" t="s">
-        <v>170</v>
-      </c>
-      <c r="R9" t="s">
-        <v>171</v>
-      </c>
-      <c r="T9" t="s">
-        <v>172</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>173</v>
-      </c>
-      <c r="AM9"/>
-      <c r="AN9" t="s">
-        <v>174</v>
-      </c>
-      <c r="AO9" t="s">
-        <v>175</v>
-      </c>
-      <c r="AP9"/>
-      <c r="AQ9"/>
-      <c r="AS9"/>
-      <c r="AT9" t="s">
-        <v>176</v>
-      </c>
-      <c r="AV9"/>
-      <c r="AX9" t="s">
-        <v>177</v>
-      </c>
-      <c r="AZ9" t="s">
-        <v>178</v>
-      </c>
-      <c r="BA9" t="s">
-        <v>179</v>
-      </c>
-      <c r="BB9" t="s">
-        <v>180</v>
-      </c>
-      <c r="BC9" t="s">
-        <v>181</v>
-      </c>
-      <c r="BD9" t="s">
-        <v>182</v>
-      </c>
-      <c r="BE9" t="s">
-        <v>183</v>
-      </c>
-      <c r="BG9" t="s">
-        <v>184</v>
-      </c>
-      <c r="BH9" t="s">
-        <v>185</v>
-      </c>
-      <c r="BI9"/>
-      <c r="BJ9" t="s">
-        <v>177</v>
-      </c>
-      <c r="BK9" t="s">
-        <v>178</v>
-      </c>
-      <c r="BL9" t="s">
-        <v>179</v>
-      </c>
-      <c r="BM9" t="s">
-        <v>186</v>
-      </c>
-      <c r="BN9" t="s">
-        <v>181</v>
-      </c>
-      <c r="BO9" t="s">
-        <v>182</v>
-      </c>
-      <c r="BP9" t="s">
-        <v>183</v>
-      </c>
-      <c r="BR9"/>
-      <c r="BT9" t="s">
-        <v>187</v>
-      </c>
-      <c r="BU9" t="s">
-        <v>261</v>
-      </c>
-      <c r="BV9" t="s">
-        <v>261</v>
-      </c>
-      <c r="BW9" t="s">
-        <v>262</v>
-      </c>
-      <c r="BX9" t="s">
-        <v>263</v>
-      </c>
-      <c r="BY9" t="s">
-        <v>191</v>
-      </c>
-      <c r="BZ9" t="s">
-        <v>192</v>
-      </c>
-      <c r="CA9" t="s">
-        <v>193</v>
-      </c>
-      <c r="CB9" t="s">
-        <v>194</v>
-      </c>
-      <c r="CC9" t="s">
-        <v>195</v>
-      </c>
-      <c r="CD9" t="s">
-        <v>196</v>
-      </c>
-      <c r="CE9" t="s">
-        <v>197</v>
-      </c>
-      <c r="CF9" t="s">
-        <v>198</v>
-      </c>
-      <c r="CG9" t="s">
-        <v>199</v>
-      </c>
-      <c r="CH9" t="s">
-        <v>200</v>
-      </c>
-      <c r="CI9" t="s">
-        <v>201</v>
-      </c>
-      <c r="CJ9" t="s">
-        <v>202</v>
-      </c>
-      <c r="CK9" t="s">
-        <v>203</v>
-      </c>
-      <c r="CL9" t="s">
-        <v>204</v>
-      </c>
-      <c r="CM9" t="s">
-        <v>205</v>
-      </c>
-      <c r="CN9" t="s">
-        <v>206</v>
-      </c>
-      <c r="CO9" t="s">
-        <v>207</v>
-      </c>
-      <c r="CP9" t="s">
-        <v>208</v>
-      </c>
-      <c r="CQ9" t="s">
-        <v>209</v>
-      </c>
-      <c r="CT9" t="s">
-        <v>264</v>
-      </c>
-      <c r="CU9" t="s">
-        <v>178</v>
-      </c>
-      <c r="CV9" t="s">
-        <v>211</v>
-      </c>
-      <c r="CW9" t="s">
-        <v>212</v>
-      </c>
-      <c r="CX9" t="s">
-        <v>182</v>
-      </c>
-      <c r="CY9" t="s">
-        <v>183</v>
-      </c>
-      <c r="CZ9" t="s">
-        <v>213</v>
-      </c>
-      <c r="DB9" t="s">
-        <v>214</v>
-      </c>
-      <c r="EB9" t="s">
-        <v>215</v>
-      </c>
-      <c r="ET9" t="s">
-        <v>160</v>
-      </c>
-      <c r="EU9" t="s">
-        <v>160</v>
-      </c>
-      <c r="EW9" t="s">
-        <v>216</v>
-      </c>
-      <c r="EX9" t="s">
-        <v>217</v>
-      </c>
-      <c r="EY9" t="s">
-        <v>218</v>
-      </c>
-      <c r="EZ9" t="s">
-        <v>219</v>
-      </c>
-      <c r="FA9" t="s">
-        <v>220</v>
-      </c>
-      <c r="FC9" t="s">
-        <v>221</v>
-      </c>
-      <c r="FD9"/>
-      <c r="FE9" t="s">
         <v>176</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Alert for client users:  added case for both cases (1. checkbox to send to all users and 2. send a specific user only)
</commit_message>
<xml_diff>
--- a/ADtests/Resources/Downloads/RF.CustomExport(BaseOfExport=Reviews)[TESTING] (1).xlsx
+++ b/ADtests/Resources/Downloads/RF.CustomExport(BaseOfExport=Reviews)[TESTING] (1).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="239">
   <si>
     <t>CritID</t>
   </si>
@@ -494,13 +494,13 @@
     <t>1108. Test custom field. Number</t>
   </si>
   <si>
-    <t>278541</t>
+    <t>278612</t>
   </si>
   <si>
     <t>46.401869158879</t>
   </si>
   <si>
-    <t>2022-09-28 10:27:53</t>
+    <t>2022-10-03 09:22:36</t>
   </si>
   <si>
     <t>RF Branch 01 [Short name]</t>
@@ -521,12 +521,18 @@
     <t>40.00</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>YES</t>
   </si>
   <si>
     <t>50.00</t>
   </si>
   <si>
+    <t>4;1</t>
+  </si>
+  <si>
     <t>Not now;Yes</t>
   </si>
   <si>
@@ -536,7 +542,10 @@
     <t>2000</t>
   </si>
   <si>
-    <t>Additional info - 28.09.2022 RF</t>
+    <t>Additional info - 03.10.2022 RF</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>green</t>
@@ -581,13 +590,13 @@
     <t>Approved</t>
   </si>
   <si>
-    <t>2022-09-28 10:28:06</t>
-  </si>
-  <si>
-    <t>2022-09-28 10:27:28</t>
-  </si>
-  <si>
-    <t>2022-09-28 10:27:02</t>
+    <t>2022-10-03 09:22:54</t>
+  </si>
+  <si>
+    <t>2022-10-03 09:22:08</t>
+  </si>
+  <si>
+    <t>2022-10-03 09:22:07</t>
   </si>
   <si>
     <t>122391</t>
@@ -647,7 +656,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>RF Order: Single_01 SMOKE [To check review status and answers, 28.09.2022]</t>
+    <t>RF Order: Single_01 SMOKE [To check review status and answers, 03.10.2022]</t>
   </si>
   <si>
     <t>TextB1</t>
@@ -683,103 +692,46 @@
     <t>"I AM a code" !@##%$</t>
   </si>
   <si>
-    <t>278542</t>
-  </si>
-  <si>
-    <t>2022-09-28 11:25:50</t>
-  </si>
-  <si>
-    <t>2022-09-28 11:26:20</t>
-  </si>
-  <si>
-    <t>2022-09-28 11:25:19</t>
-  </si>
-  <si>
-    <t>2022-09-28 11:24:53</t>
-  </si>
-  <si>
-    <t>278565</t>
-  </si>
-  <si>
-    <t>2022-09-28 23:21:58</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>4;1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>2022-09-28 23:22:13</t>
-  </si>
-  <si>
-    <t>2022-09-28 23:21:33</t>
-  </si>
-  <si>
-    <t>2022-09-28 23:21:07</t>
-  </si>
-  <si>
-    <t>278573</t>
-  </si>
-  <si>
-    <t>2022-09-29 10:44:12</t>
-  </si>
-  <si>
-    <t>Additional info - 29.09.2022 RF</t>
-  </si>
-  <si>
-    <t>2022-09-29 10:44:26</t>
-  </si>
-  <si>
-    <t>2022-09-29 10:43:47</t>
-  </si>
-  <si>
-    <t>2022-09-29 10:43:21</t>
-  </si>
-  <si>
-    <t>RF Order: Single_01 SMOKE [To check review status and answers, 29.09.2022]</t>
-  </si>
-  <si>
-    <t>278577</t>
-  </si>
-  <si>
-    <t>2022-09-29 10:59:02</t>
-  </si>
-  <si>
-    <t>2022-09-29 11:02:58</t>
-  </si>
-  <si>
-    <t>2022-09-29 10:58:36</t>
-  </si>
-  <si>
-    <t>2022-09-29 10:58:10</t>
+    <t>278623</t>
+  </si>
+  <si>
+    <t>2022-10-03 10:29:48</t>
+  </si>
+  <si>
+    <t>2022-10-03 10:30:13</t>
+  </si>
+  <si>
+    <t>2022-10-03 10:28:43</t>
+  </si>
+  <si>
+    <t>2022-10-03 10:28:42</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>RF Order: M042 [To check send repeatedly alert, 29.09.2022]</t>
+    <t>RF Order: M03 [To be accepted by a shopper and submitted with attached files, 03.10.2022]</t>
   </si>
   <si>
     <t>RF ACTIVE project 2022 [PROJECT]</t>
   </si>
   <si>
-    <t>278580</t>
-  </si>
-  <si>
-    <t>2022-09-29 12:40:43</t>
-  </si>
-  <si>
-    <t>2022-09-29 12:46:31</t>
-  </si>
-  <si>
-    <t>2022-09-29 12:40:10</t>
-  </si>
-  <si>
-    <t>2022-09-29 12:39:44</t>
+    <t>278629</t>
+  </si>
+  <si>
+    <t>2022-10-03 12:17:35</t>
+  </si>
+  <si>
+    <t>2022-10-03 12:20:26</t>
+  </si>
+  <si>
+    <t>2022-10-03 12:17:10</t>
+  </si>
+  <si>
+    <t>2022-10-03 12:17:09</t>
+  </si>
+  <si>
+    <t>RF Order: M042 [To check send repeatedly alert, 03.10.2022]</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1070,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:FG7"/>
+  <dimension ref="A1:FG4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1637,188 +1589,194 @@
       <c r="I2" t="s">
         <v>167</v>
       </c>
-      <c r="M2"/>
+      <c r="M2" t="s">
+        <v>168</v>
+      </c>
       <c r="N2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O2" t="s">
-        <v>169</v>
-      </c>
-      <c r="P2"/>
+        <v>170</v>
+      </c>
+      <c r="P2" t="s">
+        <v>171</v>
+      </c>
       <c r="Q2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="R2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="T2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AL2" t="s">
-        <v>173</v>
-      </c>
-      <c r="AM2"/>
+        <v>175</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>176</v>
+      </c>
       <c r="AN2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AO2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="AP2"/>
       <c r="AQ2"/>
       <c r="AS2"/>
       <c r="AT2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AV2"/>
       <c r="AX2" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="AZ2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="BA2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="BB2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="BC2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="BD2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="BE2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="BG2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="BH2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="BI2"/>
       <c r="BJ2" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="BK2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="BL2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="BM2" t="s">
+        <v>189</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>184</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>185</v>
+      </c>
+      <c r="BP2" t="s">
         <v>186</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>181</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>182</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>183</v>
       </c>
       <c r="BR2"/>
       <c r="BT2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="BU2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="BV2" t="s">
         <v>161</v>
       </c>
       <c r="BW2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="BX2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="BY2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="BZ2" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="CA2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="CB2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="CC2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="CD2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="CE2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="CF2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="CG2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CH2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="CI2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="CJ2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="CK2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="CL2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="CM2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="CN2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="CO2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="CP2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="CQ2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="CT2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="CU2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="CV2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="CW2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="CX2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="CY2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="CZ2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="DB2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="EB2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="ET2" t="s">
         <v>160</v>
@@ -1827,37 +1785,37 @@
         <v>160</v>
       </c>
       <c r="EW2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="EX2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="EY2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="EZ2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="FA2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="FC2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="FD2"/>
       <c r="FE2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:163">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B3" t="s">
         <v>160</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D3" t="s">
         <v>162</v>
@@ -1877,188 +1835,194 @@
       <c r="I3" t="s">
         <v>167</v>
       </c>
-      <c r="M3"/>
+      <c r="M3" t="s">
+        <v>168</v>
+      </c>
       <c r="N3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O3" t="s">
-        <v>169</v>
-      </c>
-      <c r="P3"/>
+        <v>170</v>
+      </c>
+      <c r="P3" t="s">
+        <v>171</v>
+      </c>
       <c r="Q3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="R3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="T3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AL3" t="s">
-        <v>173</v>
-      </c>
-      <c r="AM3"/>
+        <v>175</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>176</v>
+      </c>
       <c r="AN3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AO3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="AP3"/>
       <c r="AQ3"/>
       <c r="AS3"/>
       <c r="AT3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AV3"/>
       <c r="AX3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="AZ3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="BA3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="BB3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="BC3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="BD3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="BE3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="BG3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="BH3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="BI3"/>
       <c r="BJ3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="BK3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="BL3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="BM3" t="s">
+        <v>189</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>184</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>185</v>
+      </c>
+      <c r="BP3" t="s">
         <v>186</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>181</v>
-      </c>
-      <c r="BO3" t="s">
-        <v>182</v>
-      </c>
-      <c r="BP3" t="s">
-        <v>183</v>
       </c>
       <c r="BR3"/>
       <c r="BT3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="BU3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="BV3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="BW3" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="BX3" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="BY3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="BZ3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="CA3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="CB3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="CC3" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="CD3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="CE3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="CF3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="CG3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CH3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="CI3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="CJ3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="CK3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="CL3" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="CM3" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="CN3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="CO3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="CP3" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="CQ3" t="s">
-        <v>209</v>
+        <v>168</v>
       </c>
       <c r="CT3" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="CU3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="CV3" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="CW3" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="CX3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="CY3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="CZ3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="DB3" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="EB3" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="ET3" t="s">
         <v>160</v>
@@ -2067,37 +2031,40 @@
         <v>160</v>
       </c>
       <c r="EW3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="EX3" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="EY3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="EZ3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="FA3" t="s">
-        <v>220</v>
+        <v>223</v>
+      </c>
+      <c r="FB3" t="s">
+        <v>232</v>
       </c>
       <c r="FC3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="FD3"/>
       <c r="FE3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:163">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B4" t="s">
         <v>160</v>
       </c>
       <c r="C4" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="D4" t="s">
         <v>162</v>
@@ -2118,193 +2085,193 @@
         <v>167</v>
       </c>
       <c r="M4" t="s">
-        <v>229</v>
+        <v>168</v>
       </c>
       <c r="N4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="P4" t="s">
-        <v>230</v>
+        <v>171</v>
       </c>
       <c r="Q4" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="R4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="T4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AL4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AM4" t="s">
-        <v>231</v>
+        <v>176</v>
       </c>
       <c r="AN4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AO4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="AP4"/>
       <c r="AQ4"/>
       <c r="AS4"/>
       <c r="AT4" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AV4"/>
       <c r="AX4" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="AZ4" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="BA4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="BB4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="BC4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="BD4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="BE4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="BG4" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="BH4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="BI4"/>
       <c r="BJ4" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="BK4" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="BL4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="BM4" t="s">
+        <v>189</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>184</v>
+      </c>
+      <c r="BO4" t="s">
+        <v>185</v>
+      </c>
+      <c r="BP4" t="s">
         <v>186</v>
-      </c>
-      <c r="BN4" t="s">
-        <v>181</v>
-      </c>
-      <c r="BO4" t="s">
-        <v>182</v>
-      </c>
-      <c r="BP4" t="s">
-        <v>183</v>
       </c>
       <c r="BR4"/>
       <c r="BT4" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="BU4" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="BV4" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="BW4" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="BX4" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="BY4" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="BZ4" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="CA4" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="CB4" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="CC4" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="CD4" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="CE4" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="CF4" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="CG4" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CH4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="CI4" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="CJ4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="CK4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="CL4" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="CM4" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="CN4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="CO4" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="CP4" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="CQ4" t="s">
-        <v>209</v>
+        <v>168</v>
       </c>
       <c r="CT4" t="s">
-        <v>210</v>
+        <v>238</v>
       </c>
       <c r="CU4" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="CV4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="CW4" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="CX4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="CY4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="CZ4" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="DB4" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="EB4" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="ET4" t="s">
         <v>160</v>
@@ -2313,770 +2280,29 @@
         <v>160</v>
       </c>
       <c r="EW4" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="EX4" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="EY4" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="EZ4" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="FA4" t="s">
-        <v>220</v>
+        <v>223</v>
+      </c>
+      <c r="FB4" t="s">
+        <v>232</v>
       </c>
       <c r="FC4" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="FD4"/>
       <c r="FE4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:163">
-      <c r="A5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C5" t="s">
-        <v>236</v>
-      </c>
-      <c r="D5" t="s">
-        <v>162</v>
-      </c>
-      <c r="E5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F5" t="s">
-        <v>164</v>
-      </c>
-      <c r="G5" t="s">
-        <v>165</v>
-      </c>
-      <c r="H5" t="s">
-        <v>166</v>
-      </c>
-      <c r="I5" t="s">
-        <v>167</v>
-      </c>
-      <c r="M5" t="s">
-        <v>229</v>
-      </c>
-      <c r="N5" t="s">
-        <v>168</v>
-      </c>
-      <c r="O5" t="s">
-        <v>169</v>
-      </c>
-      <c r="P5" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>170</v>
-      </c>
-      <c r="R5" t="s">
-        <v>171</v>
-      </c>
-      <c r="T5" t="s">
-        <v>172</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>237</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>231</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>174</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>175</v>
-      </c>
-      <c r="AP5"/>
-      <c r="AQ5"/>
-      <c r="AS5"/>
-      <c r="AT5" t="s">
-        <v>176</v>
-      </c>
-      <c r="AV5"/>
-      <c r="AX5" t="s">
-        <v>177</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>178</v>
-      </c>
-      <c r="BA5" t="s">
         <v>179</v>
-      </c>
-      <c r="BB5" t="s">
-        <v>180</v>
-      </c>
-      <c r="BC5" t="s">
-        <v>181</v>
-      </c>
-      <c r="BD5" t="s">
-        <v>182</v>
-      </c>
-      <c r="BE5" t="s">
-        <v>183</v>
-      </c>
-      <c r="BG5" t="s">
-        <v>184</v>
-      </c>
-      <c r="BH5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BI5"/>
-      <c r="BJ5" t="s">
-        <v>177</v>
-      </c>
-      <c r="BK5" t="s">
-        <v>178</v>
-      </c>
-      <c r="BL5" t="s">
-        <v>179</v>
-      </c>
-      <c r="BM5" t="s">
-        <v>186</v>
-      </c>
-      <c r="BN5" t="s">
-        <v>181</v>
-      </c>
-      <c r="BO5" t="s">
-        <v>182</v>
-      </c>
-      <c r="BP5" t="s">
-        <v>183</v>
-      </c>
-      <c r="BR5"/>
-      <c r="BT5" t="s">
-        <v>187</v>
-      </c>
-      <c r="BU5" t="s">
-        <v>238</v>
-      </c>
-      <c r="BV5" t="s">
-        <v>236</v>
-      </c>
-      <c r="BW5" t="s">
-        <v>239</v>
-      </c>
-      <c r="BX5" t="s">
-        <v>240</v>
-      </c>
-      <c r="BY5" t="s">
-        <v>191</v>
-      </c>
-      <c r="BZ5" t="s">
-        <v>192</v>
-      </c>
-      <c r="CA5" t="s">
-        <v>193</v>
-      </c>
-      <c r="CB5" t="s">
-        <v>194</v>
-      </c>
-      <c r="CC5" t="s">
-        <v>195</v>
-      </c>
-      <c r="CD5" t="s">
-        <v>196</v>
-      </c>
-      <c r="CE5" t="s">
-        <v>197</v>
-      </c>
-      <c r="CF5" t="s">
-        <v>198</v>
-      </c>
-      <c r="CG5" t="s">
-        <v>199</v>
-      </c>
-      <c r="CH5" t="s">
-        <v>200</v>
-      </c>
-      <c r="CI5" t="s">
-        <v>201</v>
-      </c>
-      <c r="CJ5" t="s">
-        <v>202</v>
-      </c>
-      <c r="CK5" t="s">
-        <v>203</v>
-      </c>
-      <c r="CL5" t="s">
-        <v>204</v>
-      </c>
-      <c r="CM5" t="s">
-        <v>205</v>
-      </c>
-      <c r="CN5" t="s">
-        <v>206</v>
-      </c>
-      <c r="CO5" t="s">
-        <v>207</v>
-      </c>
-      <c r="CP5" t="s">
-        <v>208</v>
-      </c>
-      <c r="CQ5" t="s">
-        <v>209</v>
-      </c>
-      <c r="CT5" t="s">
-        <v>241</v>
-      </c>
-      <c r="CU5" t="s">
-        <v>178</v>
-      </c>
-      <c r="CV5" t="s">
-        <v>211</v>
-      </c>
-      <c r="CW5" t="s">
-        <v>212</v>
-      </c>
-      <c r="CX5" t="s">
-        <v>182</v>
-      </c>
-      <c r="CY5" t="s">
-        <v>183</v>
-      </c>
-      <c r="CZ5" t="s">
-        <v>213</v>
-      </c>
-      <c r="DB5" t="s">
-        <v>214</v>
-      </c>
-      <c r="EB5" t="s">
-        <v>215</v>
-      </c>
-      <c r="ET5" t="s">
-        <v>160</v>
-      </c>
-      <c r="EU5" t="s">
-        <v>160</v>
-      </c>
-      <c r="EW5" t="s">
-        <v>216</v>
-      </c>
-      <c r="EX5" t="s">
-        <v>217</v>
-      </c>
-      <c r="EY5" t="s">
-        <v>218</v>
-      </c>
-      <c r="EZ5" t="s">
-        <v>219</v>
-      </c>
-      <c r="FA5" t="s">
-        <v>220</v>
-      </c>
-      <c r="FC5" t="s">
-        <v>221</v>
-      </c>
-      <c r="FD5"/>
-      <c r="FE5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:163">
-      <c r="A6" t="s">
-        <v>242</v>
-      </c>
-      <c r="B6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C6" t="s">
-        <v>243</v>
-      </c>
-      <c r="D6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E6" t="s">
-        <v>163</v>
-      </c>
-      <c r="F6" t="s">
-        <v>164</v>
-      </c>
-      <c r="G6" t="s">
-        <v>165</v>
-      </c>
-      <c r="H6" t="s">
-        <v>166</v>
-      </c>
-      <c r="I6" t="s">
-        <v>167</v>
-      </c>
-      <c r="M6" t="s">
-        <v>229</v>
-      </c>
-      <c r="N6" t="s">
-        <v>168</v>
-      </c>
-      <c r="O6" t="s">
-        <v>169</v>
-      </c>
-      <c r="P6" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>170</v>
-      </c>
-      <c r="R6" t="s">
-        <v>171</v>
-      </c>
-      <c r="T6" t="s">
-        <v>172</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>237</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>231</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>174</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>175</v>
-      </c>
-      <c r="AP6"/>
-      <c r="AQ6"/>
-      <c r="AS6"/>
-      <c r="AT6" t="s">
-        <v>176</v>
-      </c>
-      <c r="AV6"/>
-      <c r="AX6" t="s">
-        <v>177</v>
-      </c>
-      <c r="AZ6" t="s">
-        <v>178</v>
-      </c>
-      <c r="BA6" t="s">
-        <v>179</v>
-      </c>
-      <c r="BB6" t="s">
-        <v>180</v>
-      </c>
-      <c r="BC6" t="s">
-        <v>181</v>
-      </c>
-      <c r="BD6" t="s">
-        <v>182</v>
-      </c>
-      <c r="BE6" t="s">
-        <v>183</v>
-      </c>
-      <c r="BG6" t="s">
-        <v>184</v>
-      </c>
-      <c r="BH6" t="s">
-        <v>185</v>
-      </c>
-      <c r="BI6"/>
-      <c r="BJ6" t="s">
-        <v>177</v>
-      </c>
-      <c r="BK6" t="s">
-        <v>178</v>
-      </c>
-      <c r="BL6" t="s">
-        <v>179</v>
-      </c>
-      <c r="BM6" t="s">
-        <v>186</v>
-      </c>
-      <c r="BN6" t="s">
-        <v>181</v>
-      </c>
-      <c r="BO6" t="s">
-        <v>182</v>
-      </c>
-      <c r="BP6" t="s">
-        <v>183</v>
-      </c>
-      <c r="BR6"/>
-      <c r="BT6" t="s">
-        <v>187</v>
-      </c>
-      <c r="BU6" t="s">
-        <v>244</v>
-      </c>
-      <c r="BV6" t="s">
-        <v>243</v>
-      </c>
-      <c r="BW6" t="s">
-        <v>245</v>
-      </c>
-      <c r="BX6" t="s">
-        <v>246</v>
-      </c>
-      <c r="BY6" t="s">
-        <v>191</v>
-      </c>
-      <c r="BZ6" t="s">
-        <v>192</v>
-      </c>
-      <c r="CA6" t="s">
-        <v>193</v>
-      </c>
-      <c r="CB6" t="s">
-        <v>194</v>
-      </c>
-      <c r="CC6" t="s">
-        <v>195</v>
-      </c>
-      <c r="CD6" t="s">
-        <v>196</v>
-      </c>
-      <c r="CE6" t="s">
-        <v>197</v>
-      </c>
-      <c r="CF6" t="s">
-        <v>198</v>
-      </c>
-      <c r="CG6" t="s">
-        <v>199</v>
-      </c>
-      <c r="CH6" t="s">
-        <v>200</v>
-      </c>
-      <c r="CI6" t="s">
-        <v>201</v>
-      </c>
-      <c r="CJ6" t="s">
-        <v>202</v>
-      </c>
-      <c r="CK6" t="s">
-        <v>203</v>
-      </c>
-      <c r="CL6" t="s">
-        <v>204</v>
-      </c>
-      <c r="CM6" t="s">
-        <v>205</v>
-      </c>
-      <c r="CN6" t="s">
-        <v>206</v>
-      </c>
-      <c r="CO6" t="s">
-        <v>207</v>
-      </c>
-      <c r="CP6" t="s">
-        <v>247</v>
-      </c>
-      <c r="CQ6" t="s">
-        <v>229</v>
-      </c>
-      <c r="CT6" t="s">
-        <v>248</v>
-      </c>
-      <c r="CU6" t="s">
-        <v>178</v>
-      </c>
-      <c r="CV6" t="s">
-        <v>211</v>
-      </c>
-      <c r="CW6" t="s">
-        <v>212</v>
-      </c>
-      <c r="CX6" t="s">
-        <v>182</v>
-      </c>
-      <c r="CY6" t="s">
-        <v>183</v>
-      </c>
-      <c r="CZ6" t="s">
-        <v>213</v>
-      </c>
-      <c r="DB6" t="s">
-        <v>214</v>
-      </c>
-      <c r="EB6" t="s">
-        <v>215</v>
-      </c>
-      <c r="ET6" t="s">
-        <v>160</v>
-      </c>
-      <c r="EU6" t="s">
-        <v>160</v>
-      </c>
-      <c r="EW6" t="s">
-        <v>216</v>
-      </c>
-      <c r="EX6" t="s">
-        <v>217</v>
-      </c>
-      <c r="EY6" t="s">
-        <v>218</v>
-      </c>
-      <c r="EZ6" t="s">
-        <v>219</v>
-      </c>
-      <c r="FA6" t="s">
-        <v>220</v>
-      </c>
-      <c r="FB6" t="s">
-        <v>249</v>
-      </c>
-      <c r="FC6" t="s">
-        <v>221</v>
-      </c>
-      <c r="FD6"/>
-      <c r="FE6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:163">
-      <c r="A7" t="s">
-        <v>250</v>
-      </c>
-      <c r="B7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C7" t="s">
-        <v>251</v>
-      </c>
-      <c r="D7" t="s">
-        <v>162</v>
-      </c>
-      <c r="E7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F7" t="s">
-        <v>164</v>
-      </c>
-      <c r="G7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H7" t="s">
-        <v>166</v>
-      </c>
-      <c r="I7" t="s">
-        <v>167</v>
-      </c>
-      <c r="M7" t="s">
-        <v>229</v>
-      </c>
-      <c r="N7" t="s">
-        <v>168</v>
-      </c>
-      <c r="O7" t="s">
-        <v>169</v>
-      </c>
-      <c r="P7" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>170</v>
-      </c>
-      <c r="R7" t="s">
-        <v>171</v>
-      </c>
-      <c r="T7" t="s">
-        <v>172</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>237</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>231</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>174</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>175</v>
-      </c>
-      <c r="AP7"/>
-      <c r="AQ7"/>
-      <c r="AS7"/>
-      <c r="AT7" t="s">
-        <v>176</v>
-      </c>
-      <c r="AV7"/>
-      <c r="AX7" t="s">
-        <v>177</v>
-      </c>
-      <c r="AZ7" t="s">
-        <v>178</v>
-      </c>
-      <c r="BA7" t="s">
-        <v>179</v>
-      </c>
-      <c r="BB7" t="s">
-        <v>180</v>
-      </c>
-      <c r="BC7" t="s">
-        <v>181</v>
-      </c>
-      <c r="BD7" t="s">
-        <v>182</v>
-      </c>
-      <c r="BE7" t="s">
-        <v>183</v>
-      </c>
-      <c r="BG7" t="s">
-        <v>184</v>
-      </c>
-      <c r="BH7" t="s">
-        <v>185</v>
-      </c>
-      <c r="BI7"/>
-      <c r="BJ7" t="s">
-        <v>177</v>
-      </c>
-      <c r="BK7" t="s">
-        <v>178</v>
-      </c>
-      <c r="BL7" t="s">
-        <v>179</v>
-      </c>
-      <c r="BM7" t="s">
-        <v>186</v>
-      </c>
-      <c r="BN7" t="s">
-        <v>181</v>
-      </c>
-      <c r="BO7" t="s">
-        <v>182</v>
-      </c>
-      <c r="BP7" t="s">
-        <v>183</v>
-      </c>
-      <c r="BR7"/>
-      <c r="BT7" t="s">
-        <v>187</v>
-      </c>
-      <c r="BU7" t="s">
-        <v>252</v>
-      </c>
-      <c r="BV7" t="s">
-        <v>251</v>
-      </c>
-      <c r="BW7" t="s">
-        <v>253</v>
-      </c>
-      <c r="BX7" t="s">
-        <v>254</v>
-      </c>
-      <c r="BY7" t="s">
-        <v>191</v>
-      </c>
-      <c r="BZ7" t="s">
-        <v>192</v>
-      </c>
-      <c r="CA7" t="s">
-        <v>193</v>
-      </c>
-      <c r="CB7" t="s">
-        <v>194</v>
-      </c>
-      <c r="CC7" t="s">
-        <v>195</v>
-      </c>
-      <c r="CD7" t="s">
-        <v>196</v>
-      </c>
-      <c r="CE7" t="s">
-        <v>197</v>
-      </c>
-      <c r="CF7" t="s">
-        <v>198</v>
-      </c>
-      <c r="CG7" t="s">
-        <v>199</v>
-      </c>
-      <c r="CH7" t="s">
-        <v>200</v>
-      </c>
-      <c r="CI7" t="s">
-        <v>201</v>
-      </c>
-      <c r="CJ7" t="s">
-        <v>202</v>
-      </c>
-      <c r="CK7" t="s">
-        <v>203</v>
-      </c>
-      <c r="CL7" t="s">
-        <v>204</v>
-      </c>
-      <c r="CM7" t="s">
-        <v>205</v>
-      </c>
-      <c r="CN7" t="s">
-        <v>206</v>
-      </c>
-      <c r="CO7" t="s">
-        <v>207</v>
-      </c>
-      <c r="CP7" t="s">
-        <v>247</v>
-      </c>
-      <c r="CQ7" t="s">
-        <v>229</v>
-      </c>
-      <c r="CT7" t="s">
-        <v>248</v>
-      </c>
-      <c r="CU7" t="s">
-        <v>178</v>
-      </c>
-      <c r="CV7" t="s">
-        <v>211</v>
-      </c>
-      <c r="CW7" t="s">
-        <v>212</v>
-      </c>
-      <c r="CX7" t="s">
-        <v>182</v>
-      </c>
-      <c r="CY7" t="s">
-        <v>183</v>
-      </c>
-      <c r="CZ7" t="s">
-        <v>213</v>
-      </c>
-      <c r="DB7" t="s">
-        <v>214</v>
-      </c>
-      <c r="EB7" t="s">
-        <v>215</v>
-      </c>
-      <c r="ET7" t="s">
-        <v>160</v>
-      </c>
-      <c r="EU7" t="s">
-        <v>160</v>
-      </c>
-      <c r="EW7" t="s">
-        <v>216</v>
-      </c>
-      <c r="EX7" t="s">
-        <v>217</v>
-      </c>
-      <c r="EY7" t="s">
-        <v>218</v>
-      </c>
-      <c r="EZ7" t="s">
-        <v>219</v>
-      </c>
-      <c r="FA7" t="s">
-        <v>220</v>
-      </c>
-      <c r="FB7" t="s">
-        <v>249</v>
-      </c>
-      <c r="FC7" t="s">
-        <v>221</v>
-      </c>
-      <c r="FD7"/>
-      <c r="FE7" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>